<commit_message>
multimode selection of biomarker
</commit_message>
<xml_diff>
--- a/clean_data/common_gene_cll_t2d.xlsx
+++ b/clean_data/common_gene_cll_t2d.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F731C512-A52D-483B-A25D-06C5EE428304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -226,7 +220,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -238,7 +233,9 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -259,16 +256,16 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -276,23 +273,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+  <cellXfs count="4">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -303,10 +303,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -344,69 +344,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -430,54 +432,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -487,7 +488,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -496,7 +497,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -505,7 +506,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -513,10 +514,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -545,7 +546,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -558,13 +559,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
+                <a:tint val="80000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -582,684 +582,685 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:A133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" customWidth="1"/>
+    <col min="1" max="1" style="3" width="22.719285714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="16.5">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="16.5">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="16.5">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="16.5">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="16.5">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="16.5">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="16.5">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="16.5">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="16.5">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="16.5">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="16.5">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="16.5">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="16.5">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="16.5">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="16.5">
+      <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="16.5">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="16.5">
+      <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="16.5">
+      <c r="A19" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="16.5">
+      <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="16.5">
+      <c r="A21" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="16.5">
+      <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="16.5">
+      <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="16.5">
+      <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="16.5">
+      <c r="A25" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="16.5">
+      <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="16.5">
+      <c r="A27" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="16.5">
+      <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="16.5">
+      <c r="A29" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="16.5">
+      <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="16.5">
+      <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="16.5">
+      <c r="A32" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="16.5">
+      <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="16.5">
+      <c r="A34" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="16.5">
+      <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="16.5">
+      <c r="A36" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="16.5">
+      <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="16.5">
+      <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="16.5">
+      <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="16.5">
+      <c r="A40" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="16.5">
+      <c r="A41" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="16.5">
+      <c r="A42" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="16.5">
+      <c r="A43" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="16.5">
+      <c r="A44" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="16.5">
+      <c r="A45" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="16.5">
+      <c r="A46" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="16.5">
+      <c r="A47" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="16.5">
+      <c r="A48" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="16.5">
+      <c r="A49" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="16.5">
+      <c r="A50" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="16.5">
+      <c r="A51" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="16.5">
+      <c r="A52" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="16.5">
+      <c r="A53" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="16.5">
+      <c r="A54" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="16.5">
+      <c r="A55" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="16.5">
+      <c r="A56" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="16.5">
+      <c r="A57" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="16.5">
+      <c r="A58" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="16.5">
+      <c r="A59" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="16.5">
+      <c r="A60" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="16.5">
+      <c r="A61" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="16.5">
+      <c r="A62" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="16.5">
+      <c r="A63" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="16.5">
+      <c r="A64" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="16.5">
+      <c r="A65" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="16.5">
+      <c r="A66" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="16.5">
+      <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="16.5">
+      <c r="A68" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="16.5">
+      <c r="A69" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="16.5">
+      <c r="A70" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="16.5">
+      <c r="A71" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="16.5">
+      <c r="A72" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="16.5">
+      <c r="A73" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="16.5">
+      <c r="A74" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="16.5">
+      <c r="A75" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="16.5">
+      <c r="A76" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="16.5">
+      <c r="A77" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="16.5">
+      <c r="A78" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="16.5">
+      <c r="A79" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="16.5">
+      <c r="A80" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="16.5">
+      <c r="A81" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="16.5">
+      <c r="A82" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="16.5">
+      <c r="A83" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="16.5">
+      <c r="A84" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="16.5">
+      <c r="A85" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="16.5">
+      <c r="A86" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="16.5">
+      <c r="A87" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="16.5">
+      <c r="A88" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="16.5">
+      <c r="A89" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="16.5">
+      <c r="A90" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="16.5">
+      <c r="A91" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="16.5">
+      <c r="A92" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="16.5">
+      <c r="A93" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="16.5">
+      <c r="A94" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="16.5">
+      <c r="A95" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="16.5">
+      <c r="A96" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="16.5">
+      <c r="A97" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="16.5">
+      <c r="A98" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="16.5">
+      <c r="A99" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="16.5">
+      <c r="A100" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="16.5">
+      <c r="A101" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="16.5">
+      <c r="A102" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="16.5">
+      <c r="A103" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="16.5">
+      <c r="A104" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="16.5">
+      <c r="A105" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="16.5">
+      <c r="A106" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="16.5">
+      <c r="A107" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="16.5">
+      <c r="A108" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="16.5">
+      <c r="A109" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="16.5">
+      <c r="A110" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="16.5">
+      <c r="A111" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
+    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="16.5">
+      <c r="A112" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
+    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="16.5">
+      <c r="A113" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="16.5">
+      <c r="A114" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
+    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="16.5">
+      <c r="A115" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
+    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="16.5">
+      <c r="A116" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
+    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="16.5">
+      <c r="A117" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
+    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="16.5">
+      <c r="A118" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
+    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="16.5">
+      <c r="A119" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
+    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="16.5">
+      <c r="A120" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A121" t="s">
+    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="16.5">
+      <c r="A121" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A122" t="s">
+    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="16.5">
+      <c r="A122" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A123" t="s">
+    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="16.5">
+      <c r="A123" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
+    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="16.5">
+      <c r="A124" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A125" t="s">
+    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="16.5">
+      <c r="A125" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A126" t="s">
+    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="16.5">
+      <c r="A126" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
+    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="16.5">
+      <c r="A127" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
+    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="16.5">
+      <c r="A128" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
+    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="16.5">
+      <c r="A129" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130" t="s">
+    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="16.5">
+      <c r="A130" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A131" t="s">
+    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="16.5">
+      <c r="A131" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
+    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="16.5">
+      <c r="A132" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
+    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="16.5">
+      <c r="A133" s="2" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>